<commit_message>
update quarter date format
</commit_message>
<xml_diff>
--- a/datasets/productivity/labor_productivity_reformat.xlsx
+++ b/datasets/productivity/labor_productivity_reformat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wye\Documents\UIUC MCS\CS498\Create a narrative visualization\CS498NarrativeVisualization\datasets\productivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B492B1D-E0BE-407A-8AA3-ED8FA332FF50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A3AFA2-AF82-40C9-8BEC-0937FB9AF4BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="24900" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="1470" windowWidth="24900" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,129 +100,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>Qtr1-2010</t>
-  </si>
-  <si>
-    <t>Qtr2-2010</t>
-  </si>
-  <si>
-    <t>Qtr1-2011</t>
-  </si>
-  <si>
-    <t>Qtr1-2012</t>
-  </si>
-  <si>
-    <t>Qtr1-2013</t>
-  </si>
-  <si>
-    <t>Qtr1-2014</t>
-  </si>
-  <si>
-    <t>Qtr1-2015</t>
-  </si>
-  <si>
-    <t>Qtr1-2016</t>
-  </si>
-  <si>
-    <t>Qtr1-2017</t>
-  </si>
-  <si>
-    <t>Qtr1-2018</t>
-  </si>
-  <si>
-    <t>Qtr1-2019</t>
-  </si>
-  <si>
-    <t>Qtr1-2020</t>
-  </si>
-  <si>
-    <t>Qtr2-2011</t>
-  </si>
-  <si>
-    <t>Qtr2-2012</t>
-  </si>
-  <si>
-    <t>Qtr2-2013</t>
-  </si>
-  <si>
-    <t>Qtr2-2014</t>
-  </si>
-  <si>
-    <t>Qtr2-2015</t>
-  </si>
-  <si>
-    <t>Qtr2-2016</t>
-  </si>
-  <si>
-    <t>Qtr2-2017</t>
-  </si>
-  <si>
-    <t>Qtr2-2018</t>
-  </si>
-  <si>
-    <t>Qtr2-2019</t>
-  </si>
-  <si>
-    <t>Qtr3-2010</t>
-  </si>
-  <si>
-    <t>Qtr3-2011</t>
-  </si>
-  <si>
-    <t>Qtr3-2012</t>
-  </si>
-  <si>
-    <t>Qtr3-2013</t>
-  </si>
-  <si>
-    <t>Qtr3-2014</t>
-  </si>
-  <si>
-    <t>Qtr3-2015</t>
-  </si>
-  <si>
-    <t>Qtr3-2016</t>
-  </si>
-  <si>
-    <t>Qtr3-2017</t>
-  </si>
-  <si>
-    <t>Qtr3-2018</t>
-  </si>
-  <si>
-    <t>Qtr3-2019</t>
-  </si>
-  <si>
-    <t>Qtr4-2010</t>
-  </si>
-  <si>
-    <t>Qtr4-2011</t>
-  </si>
-  <si>
-    <t>Qtr4-2012</t>
-  </si>
-  <si>
-    <t>Qtr4-2013</t>
-  </si>
-  <si>
-    <t>Qtr4-2014</t>
-  </si>
-  <si>
-    <t>Qtr4-2015</t>
-  </si>
-  <si>
-    <t>Qtr4-2016</t>
-  </si>
-  <si>
-    <t>Qtr4-2017</t>
-  </si>
-  <si>
-    <t>Qtr4-2018</t>
-  </si>
-  <si>
-    <t>Qtr4-2019</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
@@ -230,6 +107,129 @@
   </si>
   <si>
     <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>1-2010</t>
+  </si>
+  <si>
+    <t>2-2010</t>
+  </si>
+  <si>
+    <t>1-2011</t>
+  </si>
+  <si>
+    <t>2-2011</t>
+  </si>
+  <si>
+    <t>3-2010</t>
+  </si>
+  <si>
+    <t>4-2010</t>
+  </si>
+  <si>
+    <t>3-2011</t>
+  </si>
+  <si>
+    <t>4-2011</t>
+  </si>
+  <si>
+    <t>1-2012</t>
+  </si>
+  <si>
+    <t>2-2012</t>
+  </si>
+  <si>
+    <t>3-2012</t>
+  </si>
+  <si>
+    <t>4-2012</t>
+  </si>
+  <si>
+    <t>1-2013</t>
+  </si>
+  <si>
+    <t>2-2013</t>
+  </si>
+  <si>
+    <t>3-2013</t>
+  </si>
+  <si>
+    <t>4-2013</t>
+  </si>
+  <si>
+    <t>1-2014</t>
+  </si>
+  <si>
+    <t>2-2014</t>
+  </si>
+  <si>
+    <t>3-2014</t>
+  </si>
+  <si>
+    <t>4-2014</t>
+  </si>
+  <si>
+    <t>1-2015</t>
+  </si>
+  <si>
+    <t>2-2015</t>
+  </si>
+  <si>
+    <t>3-2015</t>
+  </si>
+  <si>
+    <t>4-2015</t>
+  </si>
+  <si>
+    <t>1-2016</t>
+  </si>
+  <si>
+    <t>2-2016</t>
+  </si>
+  <si>
+    <t>3-2016</t>
+  </si>
+  <si>
+    <t>4-2016</t>
+  </si>
+  <si>
+    <t>1-2017</t>
+  </si>
+  <si>
+    <t>2-2017</t>
+  </si>
+  <si>
+    <t>3-2017</t>
+  </si>
+  <si>
+    <t>4-2017</t>
+  </si>
+  <si>
+    <t>1-2018</t>
+  </si>
+  <si>
+    <t>2-2018</t>
+  </si>
+  <si>
+    <t>3-2018</t>
+  </si>
+  <si>
+    <t>4-2018</t>
+  </si>
+  <si>
+    <t>1-2019</t>
+  </si>
+  <si>
+    <t>2-2019</t>
+  </si>
+  <si>
+    <t>3-2019</t>
+  </si>
+  <si>
+    <t>4-2019</t>
+  </si>
+  <si>
+    <t>1-2020</t>
   </si>
 </sst>
 </file>
@@ -239,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +268,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -604,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,18 +625,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
         <v>1.4</v>
@@ -644,7 +650,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <v>0.9</v>
@@ -658,7 +664,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6">
         <v>2.4</v>
@@ -672,7 +678,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6">
         <v>1.1000000000000001</v>
@@ -686,7 +692,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6">
         <v>-3</v>
@@ -700,7 +706,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B7" s="6">
         <v>0.7</v>
@@ -714,7 +720,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6">
         <v>-1.6</v>
@@ -728,7 +734,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6">
         <v>2.8</v>
@@ -742,7 +748,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6">
         <v>1.1000000000000001</v>
@@ -756,7 +762,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6">
         <v>1.7</v>
@@ -770,7 +776,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6">
         <v>-1</v>
@@ -784,7 +790,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B13" s="6">
         <v>-1.2</v>
@@ -798,7 +804,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B14" s="6">
         <v>3.7</v>
@@ -812,7 +818,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6">
         <v>-0.7</v>
@@ -826,7 +832,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B16" s="6">
         <v>1.6</v>
@@ -840,7 +846,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B17" s="6">
         <v>2.8</v>
@@ -854,7 +860,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B18" s="6">
         <v>-3.6</v>
@@ -868,7 +874,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B19" s="6">
         <v>4</v>
@@ -882,7 +888,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" s="6">
         <v>3.3</v>
@@ -896,7 +902,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B21" s="6">
         <v>-2.1</v>
@@ -910,7 +916,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B22" s="6">
         <v>2.7</v>
@@ -924,7 +930,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B23" s="6">
         <v>2</v>
@@ -938,7 +944,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="6">
         <v>1</v>
@@ -952,7 +958,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B25" s="6">
         <v>-3</v>
@@ -966,7 +972,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B26" s="6">
         <v>0.6</v>
@@ -980,7 +986,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B27" s="6">
         <v>0.6</v>
@@ -994,7 +1000,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" s="6">
         <v>1.6</v>
@@ -1008,7 +1014,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B29" s="6">
         <v>2.4</v>
@@ -1022,7 +1028,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B30" s="6">
         <v>0.7</v>
@@ -1036,7 +1042,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B31" s="6">
         <v>0.5</v>
@@ -1050,7 +1056,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B32" s="6">
         <v>3.3</v>
@@ -1064,7 +1070,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B33" s="6">
         <v>0.1</v>
@@ -1078,7 +1084,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6">
         <v>1.3</v>
@@ -1092,7 +1098,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B35" s="6">
         <v>2.7</v>
@@ -1106,7 +1112,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B36" s="6">
         <v>1.3</v>
@@ -1120,7 +1126,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="6">
         <v>0.4</v>
@@ -1134,7 +1140,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6">
         <v>4</v>
@@ -1148,7 +1154,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B39" s="6">
         <v>3</v>
@@ -1162,7 +1168,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6">
         <v>-0.4</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B41" s="6">
         <v>1</v>
@@ -1190,7 +1196,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B42" s="6">
         <v>-0.7</v>
@@ -1203,6 +1209,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>